<commit_message>
local convertion of front-end
</commit_message>
<xml_diff>
--- a/public/assets/Leads.xlsx
+++ b/public/assets/Leads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Formation\Desktop\new\front\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12853E25-B962-4740-A17B-CAB1883C9C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7B8FD9-90E7-4F1F-A7D8-B95F82CCA7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26265" yWindow="4275" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>First_Name</t>
-  </si>
-  <si>
-    <t>Last_Name</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>referral email</t>
   </si>
 </sst>
 </file>
@@ -360,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -372,29 +390,50 @@
     <col min="2" max="2" width="18.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>